<commit_message>
feature: parsing works fine
</commit_message>
<xml_diff>
--- a/SLR.xlsx
+++ b/SLR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihun-ui/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\0_CAU\3-1\Compiler\SLR_parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE770B17-6132-CA4D-8772-5F3854DC2D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A3237B-ABBC-494B-A7A5-E8036AF99DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{51119902-B807-DB44-9B77-4DF7F38F65F2}"/>
+    <workbookView xWindow="29160" yWindow="390" windowWidth="9240" windowHeight="15810" xr2:uid="{51119902-B807-DB44-9B77-4DF7F38F65F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1193,12 +1193,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1232,7 +1232,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1281,7 +1281,9 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{7612C679-4F17-4DA2-A406-9FA139A95F5F}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1612,13 +1614,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701564E2-F7EF-5D4C-9FD6-2286C92C86D1}">
   <dimension ref="A1:AL76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView tabSelected="1" topLeftCell="U18" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="V67" sqref="V67:V72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -1734,7 +1736,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1786,7 +1788,7 @@
       <c r="AK2" s="3"/>
       <c r="AL2" s="3"/>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1830,7 +1832,7 @@
       <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1882,7 +1884,7 @@
       <c r="AK4" s="3"/>
       <c r="AL4" s="3"/>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1934,7 +1936,7 @@
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1980,7 +1982,7 @@
       <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2024,7 +2026,7 @@
       <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -2068,7 +2070,7 @@
       <c r="AK8" s="3"/>
       <c r="AL8" s="3"/>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -2116,7 +2118,7 @@
       <c r="AK9" s="3"/>
       <c r="AL9" s="3"/>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -2160,7 +2162,7 @@
       <c r="AK10" s="3"/>
       <c r="AL10" s="3"/>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -2216,7 +2218,7 @@
       <c r="AK11" s="3"/>
       <c r="AL11" s="3"/>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -2264,7 +2266,7 @@
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2324,7 +2326,7 @@
       <c r="AK13" s="3"/>
       <c r="AL13" s="3"/>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -2380,7 +2382,7 @@
       <c r="AK14" s="3"/>
       <c r="AL14" s="3"/>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -2424,7 +2426,7 @@
       <c r="AK15" s="3"/>
       <c r="AL15" s="3"/>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -2468,7 +2470,7 @@
       <c r="AK16" s="3"/>
       <c r="AL16" s="3"/>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2512,7 +2514,7 @@
       <c r="AK17" s="3"/>
       <c r="AL17" s="3"/>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -2556,7 +2558,7 @@
       <c r="AK18" s="3"/>
       <c r="AL18" s="3"/>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2600,7 +2602,7 @@
       <c r="AK19" s="3"/>
       <c r="AL19" s="3"/>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2644,7 +2646,7 @@
       <c r="AK20" s="3"/>
       <c r="AL20" s="3"/>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2688,7 +2690,7 @@
       <c r="AK21" s="3"/>
       <c r="AL21" s="3"/>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2736,7 +2738,7 @@
       <c r="AK22" s="3"/>
       <c r="AL22" s="3"/>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2786,7 +2788,7 @@
       <c r="AK23" s="3"/>
       <c r="AL23" s="3"/>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2836,7 +2838,7 @@
       <c r="AK24" s="3"/>
       <c r="AL24" s="3"/>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2886,7 +2888,7 @@
       <c r="AK25" s="3"/>
       <c r="AL25" s="3"/>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2930,7 +2932,7 @@
       <c r="AK26" s="3"/>
       <c r="AL26" s="3"/>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2978,7 +2980,7 @@
       <c r="AK27" s="3"/>
       <c r="AL27" s="3"/>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3030,7 +3032,7 @@
       <c r="AK28" s="3"/>
       <c r="AL28" s="3"/>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -3082,7 +3084,7 @@
       <c r="AK29" s="3"/>
       <c r="AL29" s="3"/>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -3126,7 +3128,7 @@
       <c r="AK30" s="3"/>
       <c r="AL30" s="3"/>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -3188,7 +3190,7 @@
       <c r="AK31" s="3"/>
       <c r="AL31" s="3"/>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -3232,7 +3234,7 @@
       <c r="AK32" s="3"/>
       <c r="AL32" s="3"/>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -3276,7 +3278,7 @@
       <c r="AK33" s="3"/>
       <c r="AL33" s="3"/>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -3320,7 +3322,7 @@
       <c r="AK34" s="3"/>
       <c r="AL34" s="3"/>
     </row>
-    <row r="35" spans="1:38">
+    <row r="35" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -3364,7 +3366,7 @@
       <c r="AK35" s="3"/>
       <c r="AL35" s="3"/>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -3414,7 +3416,7 @@
       <c r="AK36" s="3"/>
       <c r="AL36" s="3"/>
     </row>
-    <row r="37" spans="1:38">
+    <row r="37" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -3460,7 +3462,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:38">
+    <row r="38" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -3522,7 +3524,7 @@
       <c r="AK38" s="3"/>
       <c r="AL38" s="3"/>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -3576,7 +3578,7 @@
       <c r="AK39" s="3"/>
       <c r="AL39" s="3"/>
     </row>
-    <row r="40" spans="1:38">
+    <row r="40" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -3620,7 +3622,7 @@
       <c r="AK40" s="3"/>
       <c r="AL40" s="3"/>
     </row>
-    <row r="41" spans="1:38">
+    <row r="41" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -3664,7 +3666,7 @@
       <c r="AK41" s="3"/>
       <c r="AL41" s="3"/>
     </row>
-    <row r="42" spans="1:38">
+    <row r="42" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -3708,7 +3710,7 @@
       <c r="AK42" s="3"/>
       <c r="AL42" s="3"/>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -3754,7 +3756,7 @@
       <c r="AK43" s="3"/>
       <c r="AL43" s="3"/>
     </row>
-    <row r="44" spans="1:38">
+    <row r="44" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -3798,7 +3800,7 @@
       <c r="AK44" s="3"/>
       <c r="AL44" s="3"/>
     </row>
-    <row r="45" spans="1:38">
+    <row r="45" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -3842,7 +3844,7 @@
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
     </row>
-    <row r="46" spans="1:38">
+    <row r="46" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -3886,7 +3888,7 @@
       <c r="AK46" s="3"/>
       <c r="AL46" s="3"/>
     </row>
-    <row r="47" spans="1:38">
+    <row r="47" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -3946,7 +3948,7 @@
       <c r="AK47" s="3"/>
       <c r="AL47" s="3"/>
     </row>
-    <row r="48" spans="1:38">
+    <row r="48" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -3992,7 +3994,7 @@
       <c r="AK48" s="3"/>
       <c r="AL48" s="3"/>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -4046,7 +4048,7 @@
       <c r="AK49" s="3"/>
       <c r="AL49" s="3"/>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -4094,7 +4096,7 @@
       <c r="AK50" s="3"/>
       <c r="AL50" s="3"/>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -4142,7 +4144,7 @@
       <c r="AK51" s="3"/>
       <c r="AL51" s="3"/>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -4188,7 +4190,7 @@
       <c r="AK52" s="3"/>
       <c r="AL52" s="3"/>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
         <v>51</v>
       </c>
@@ -4236,7 +4238,7 @@
       <c r="AK53" s="3"/>
       <c r="AL53" s="3"/>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -4282,7 +4284,7 @@
       <c r="AK54" s="3"/>
       <c r="AL54" s="3"/>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -4326,7 +4328,7 @@
       <c r="AK55" s="3"/>
       <c r="AL55" s="3"/>
     </row>
-    <row r="56" spans="1:38">
+    <row r="56" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -4372,7 +4374,7 @@
       <c r="AK56" s="3"/>
       <c r="AL56" s="3"/>
     </row>
-    <row r="57" spans="1:38">
+    <row r="57" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -4418,7 +4420,7 @@
       <c r="AK57" s="3"/>
       <c r="AL57" s="3"/>
     </row>
-    <row r="58" spans="1:38">
+    <row r="58" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -4464,7 +4466,7 @@
       <c r="AK58" s="3"/>
       <c r="AL58" s="3"/>
     </row>
-    <row r="59" spans="1:38">
+    <row r="59" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -4510,7 +4512,7 @@
       <c r="AK59" s="3"/>
       <c r="AL59" s="3"/>
     </row>
-    <row r="60" spans="1:38">
+    <row r="60" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -4554,7 +4556,7 @@
       <c r="AK60" s="3"/>
       <c r="AL60" s="3"/>
     </row>
-    <row r="61" spans="1:38">
+    <row r="61" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -4598,7 +4600,7 @@
       <c r="AK61" s="3"/>
       <c r="AL61" s="3"/>
     </row>
-    <row r="62" spans="1:38">
+    <row r="62" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -4642,7 +4644,7 @@
       <c r="AK62" s="3"/>
       <c r="AL62" s="3"/>
     </row>
-    <row r="63" spans="1:38">
+    <row r="63" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -4688,7 +4690,7 @@
       <c r="AK63" s="3"/>
       <c r="AL63" s="3"/>
     </row>
-    <row r="64" spans="1:38">
+    <row r="64" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -4732,7 +4734,7 @@
       <c r="AK64" s="3"/>
       <c r="AL64" s="3"/>
     </row>
-    <row r="65" spans="1:38">
+    <row r="65" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -4794,7 +4796,7 @@
       <c r="AK65" s="3"/>
       <c r="AL65" s="3"/>
     </row>
-    <row r="66" spans="1:38">
+    <row r="66" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -4840,7 +4842,7 @@
       <c r="AK66" s="3"/>
       <c r="AL66" s="3"/>
     </row>
-    <row r="67" spans="1:38">
+    <row r="67" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -4902,7 +4904,7 @@
       <c r="AK67" s="3"/>
       <c r="AL67" s="3"/>
     </row>
-    <row r="68" spans="1:38">
+    <row r="68" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -4946,7 +4948,7 @@
       <c r="AK68" s="3"/>
       <c r="AL68" s="3"/>
     </row>
-    <row r="69" spans="1:38">
+    <row r="69" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A69" s="2">
         <v>67</v>
       </c>
@@ -4990,7 +4992,7 @@
       <c r="AK69" s="3"/>
       <c r="AL69" s="3"/>
     </row>
-    <row r="70" spans="1:38">
+    <row r="70" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -5030,7 +5032,6 @@
       </c>
       <c r="V70" s="3"/>
       <c r="W70" s="3"/>
-      <c r="X70" s="3"/>
       <c r="Y70" s="3"/>
       <c r="Z70" s="3"/>
       <c r="AA70" s="3"/>
@@ -5048,7 +5049,7 @@
       </c>
       <c r="AL70" s="3"/>
     </row>
-    <row r="71" spans="1:38">
+    <row r="71" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A71" s="2">
         <v>69</v>
       </c>
@@ -5102,7 +5103,7 @@
       <c r="AK71" s="3"/>
       <c r="AL71" s="3"/>
     </row>
-    <row r="72" spans="1:38">
+    <row r="72" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -5156,7 +5157,7 @@
       <c r="AK72" s="3"/>
       <c r="AL72" s="3"/>
     </row>
-    <row r="73" spans="1:38">
+    <row r="73" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -5200,7 +5201,7 @@
       <c r="AK73" s="3"/>
       <c r="AL73" s="3"/>
     </row>
-    <row r="74" spans="1:38">
+    <row r="74" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -5262,7 +5263,7 @@
       <c r="AK74" s="3"/>
       <c r="AL74" s="3"/>
     </row>
-    <row r="75" spans="1:38">
+    <row r="75" spans="1:38" ht="15" x14ac:dyDescent="0.15">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -5306,7 +5307,7 @@
       <c r="AK75" s="3"/>
       <c r="AL75" s="3"/>
     </row>
-    <row r="76" spans="1:38">
+    <row r="76" spans="1:38" ht="18" x14ac:dyDescent="0.15">
       <c r="A76" s="2">
         <v>74</v>
       </c>

</xml_diff>